<commit_message>
added new API endpoint to predict players
</commit_message>
<xml_diff>
--- a/Statistics/Historical/evaluation.xlsx
+++ b/Statistics/Historical/evaluation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Moneyball\MoneyBall_Code\Statistics\Historical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602FCDEC-FA7F-41B2-A67B-980BA3C0C061}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51291C-29EB-4D18-A7D1-57B1735ED32B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{DDEA805C-D17E-4AF5-9BCD-4D2761012DB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DDEA805C-D17E-4AF5-9BCD-4D2761012DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="gbm_rf" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>None</t>
   </si>
@@ -176,6 +177,21 @@
   </si>
   <si>
     <t>No Text/Betting Data</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>GBM_3</t>
+  </si>
+  <si>
+    <t>RF_Fix</t>
+  </si>
+  <si>
+    <t>Random Forests</t>
+  </si>
+  <si>
+    <t>Gradient Boosting Machines</t>
   </si>
 </sst>
 </file>
@@ -3018,6 +3034,881 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Comparing Random Forest</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> to GBM performance in 2018/19 Season</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gbm_rf!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random Forests</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-DE7F-4C05-8B42-E3424F0F98B5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>gbm_rf!$G$2:$G$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>615</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>694</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>881</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>942</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1089</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1143</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1198</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1264</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1393</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1466</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1608</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1726</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1772</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1894</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2162</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE7F-4C05-8B42-E3424F0F98B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gbm_rf!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gradient Boosting Machines</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-DE7F-4C05-8B42-E3424F0F98B5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>gbm_rf!$H$2:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>779</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>853</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>975</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1190</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1255</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1299</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1361</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1423</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1554</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1706</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1784</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1838</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1896</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2137</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2190</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2254</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2328</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE7F-4C05-8B42-E3424F0F98B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="555609168"/>
+        <c:axId val="555612048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="555609168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Gameweek</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555612048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="555612048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555609168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3098,6 +3989,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4130,6 +5061,509 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4196,6 +5630,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A1FA5BF-2B48-4648-B1A6-2CF9B7F981E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794D65F4-BEA0-4470-A8D0-4BB26D78DB0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5155,7 +6630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC83034-E841-4EEC-82D4-C19F408BA94D}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
@@ -6227,4 +7702,925 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD529F2-74D2-412E-8B56-7C86EFC7D0AC}">
+  <dimension ref="A1:H38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>69</v>
+      </c>
+      <c r="B2">
+        <f>A2-10</f>
+        <v>59</v>
+      </c>
+      <c r="C2">
+        <f xml:space="preserve"> D2-10</f>
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <f>SUM($C$2:$C2)</f>
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <f>SUM($B$2:$B2)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>72</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B38" si="0">A3-10</f>
+        <v>62</v>
+      </c>
+      <c r="C3">
+        <f xml:space="preserve"> D3-10</f>
+        <v>62</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+      <c r="G3">
+        <f>SUM($C$2:$C3)</f>
+        <v>112</v>
+      </c>
+      <c r="H3">
+        <f>SUM($B$2:$B3)</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <f xml:space="preserve"> D4-10</f>
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>52</v>
+      </c>
+      <c r="G4">
+        <f>SUM($C$2:$C4)</f>
+        <v>154</v>
+      </c>
+      <c r="H4">
+        <f>SUM($B$2:$B4)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <f xml:space="preserve"> D5-10</f>
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <f>SUM($C$2:$C5)</f>
+        <v>203</v>
+      </c>
+      <c r="H5">
+        <f>SUM($B$2:$B5)</f>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>81</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="C6">
+        <f xml:space="preserve"> D6-10</f>
+        <v>67</v>
+      </c>
+      <c r="D6">
+        <v>77</v>
+      </c>
+      <c r="G6">
+        <f>SUM($C$2:$C6)</f>
+        <v>270</v>
+      </c>
+      <c r="H6">
+        <f>SUM($B$2:$B6)</f>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>94</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <f xml:space="preserve"> D7-10</f>
+        <v>63</v>
+      </c>
+      <c r="D7">
+        <v>73</v>
+      </c>
+      <c r="G7">
+        <f>SUM($C$2:$C7)</f>
+        <v>333</v>
+      </c>
+      <c r="H7">
+        <f>SUM($B$2:$B7)</f>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>85</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <f xml:space="preserve"> D8-10</f>
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>73</v>
+      </c>
+      <c r="G8">
+        <f>SUM($C$2:$C8)</f>
+        <v>396</v>
+      </c>
+      <c r="H8">
+        <f>SUM($B$2:$B8)</f>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>82</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="C9">
+        <f xml:space="preserve"> D9-10</f>
+        <v>47</v>
+      </c>
+      <c r="D9">
+        <v>57</v>
+      </c>
+      <c r="G9">
+        <f>SUM($C$2:$C9)</f>
+        <v>443</v>
+      </c>
+      <c r="H9">
+        <f>SUM($B$2:$B9)</f>
+        <v>539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C10">
+        <f xml:space="preserve"> D10-10</f>
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <f>SUM($C$2:$C10)</f>
+        <v>503</v>
+      </c>
+      <c r="H10">
+        <f>SUM($B$2:$B10)</f>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <f xml:space="preserve"> D11-10</f>
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <f>SUM($C$2:$C11)</f>
+        <v>557</v>
+      </c>
+      <c r="H11">
+        <f>SUM($B$2:$B11)</f>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>73</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <f xml:space="preserve"> D12-10</f>
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <f>SUM($C$2:$C12)</f>
+        <v>615</v>
+      </c>
+      <c r="H12">
+        <f>SUM($B$2:$B12)</f>
+        <v>707</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="C13">
+        <f xml:space="preserve"> D13-10</f>
+        <v>79</v>
+      </c>
+      <c r="D13">
+        <v>89</v>
+      </c>
+      <c r="G13">
+        <f>SUM($C$2:$C13)</f>
+        <v>694</v>
+      </c>
+      <c r="H13">
+        <f>SUM($B$2:$B13)</f>
+        <v>779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>84</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="C14">
+        <f xml:space="preserve"> D14-10</f>
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>70</v>
+      </c>
+      <c r="G14">
+        <f>SUM($C$2:$C14)</f>
+        <v>754</v>
+      </c>
+      <c r="H14">
+        <f>SUM($B$2:$B14)</f>
+        <v>853</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <f xml:space="preserve"> D15-10</f>
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>59</v>
+      </c>
+      <c r="G15">
+        <f>SUM($C$2:$C15)</f>
+        <v>803</v>
+      </c>
+      <c r="H15">
+        <f>SUM($B$2:$B15)</f>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>82</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="C16">
+        <f xml:space="preserve"> D16-10</f>
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>88</v>
+      </c>
+      <c r="G16">
+        <f>SUM($C$2:$C16)</f>
+        <v>881</v>
+      </c>
+      <c r="H16">
+        <f>SUM($B$2:$B16)</f>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C17">
+        <f xml:space="preserve"> D17-10</f>
+        <v>61</v>
+      </c>
+      <c r="D17">
+        <v>71</v>
+      </c>
+      <c r="G17">
+        <f>SUM($C$2:$C17)</f>
+        <v>942</v>
+      </c>
+      <c r="H17">
+        <f>SUM($B$2:$B17)</f>
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>91</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="C18">
+        <f xml:space="preserve"> D18-10</f>
+        <v>75</v>
+      </c>
+      <c r="D18">
+        <v>85</v>
+      </c>
+      <c r="G18">
+        <f>SUM($C$2:$C18)</f>
+        <v>1017</v>
+      </c>
+      <c r="H18">
+        <f>SUM($B$2:$B18)</f>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>79</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C19">
+        <f xml:space="preserve"> D19-10</f>
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>82</v>
+      </c>
+      <c r="G19">
+        <f>SUM($C$2:$C19)</f>
+        <v>1089</v>
+      </c>
+      <c r="H19">
+        <f>SUM($B$2:$B19)</f>
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C20">
+        <f xml:space="preserve"> D20-10</f>
+        <v>54</v>
+      </c>
+      <c r="D20">
+        <v>64</v>
+      </c>
+      <c r="G20">
+        <f>SUM($C$2:$C20)</f>
+        <v>1143</v>
+      </c>
+      <c r="H20">
+        <f>SUM($B$2:$B20)</f>
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>54</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C21">
+        <f xml:space="preserve"> D21-10</f>
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>65</v>
+      </c>
+      <c r="G21">
+        <f>SUM($C$2:$C21)</f>
+        <v>1198</v>
+      </c>
+      <c r="H21">
+        <f>SUM($B$2:$B21)</f>
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="C22">
+        <f xml:space="preserve"> D22-10</f>
+        <v>66</v>
+      </c>
+      <c r="D22">
+        <v>76</v>
+      </c>
+      <c r="G22">
+        <f>SUM($C$2:$C22)</f>
+        <v>1264</v>
+      </c>
+      <c r="H22">
+        <f>SUM($B$2:$B22)</f>
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>72</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="C23">
+        <f xml:space="preserve"> D23-10</f>
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>77</v>
+      </c>
+      <c r="G23">
+        <f>SUM($C$2:$C23)</f>
+        <v>1331</v>
+      </c>
+      <c r="H23">
+        <f>SUM($B$2:$B23)</f>
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>75</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <f xml:space="preserve"> D24-10</f>
+        <v>62</v>
+      </c>
+      <c r="D24">
+        <v>72</v>
+      </c>
+      <c r="G24">
+        <f>SUM($C$2:$C24)</f>
+        <v>1393</v>
+      </c>
+      <c r="H24">
+        <f>SUM($B$2:$B24)</f>
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>76</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="C25">
+        <f xml:space="preserve"> D25-10</f>
+        <v>73</v>
+      </c>
+      <c r="D25">
+        <v>83</v>
+      </c>
+      <c r="G25">
+        <f>SUM($C$2:$C25)</f>
+        <v>1466</v>
+      </c>
+      <c r="H25">
+        <f>SUM($B$2:$B25)</f>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>88</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="C26">
+        <f xml:space="preserve"> D26-10</f>
+        <v>74</v>
+      </c>
+      <c r="D26">
+        <v>84</v>
+      </c>
+      <c r="G26">
+        <f>SUM($C$2:$C26)</f>
+        <v>1540</v>
+      </c>
+      <c r="H26">
+        <f>SUM($B$2:$B26)</f>
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>84</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="C27">
+        <f xml:space="preserve"> D27-10</f>
+        <v>68</v>
+      </c>
+      <c r="D27">
+        <v>78</v>
+      </c>
+      <c r="G27">
+        <f>SUM($C$2:$C27)</f>
+        <v>1608</v>
+      </c>
+      <c r="H27">
+        <f>SUM($B$2:$B27)</f>
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>88</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="C28">
+        <f xml:space="preserve"> D28-10</f>
+        <v>72</v>
+      </c>
+      <c r="D28">
+        <v>82</v>
+      </c>
+      <c r="G28">
+        <f>SUM($C$2:$C28)</f>
+        <v>1680</v>
+      </c>
+      <c r="H28">
+        <f>SUM($B$2:$B28)</f>
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>64</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C29">
+        <f xml:space="preserve"> D29-10</f>
+        <v>46</v>
+      </c>
+      <c r="D29">
+        <v>56</v>
+      </c>
+      <c r="G29">
+        <f>SUM($C$2:$C29)</f>
+        <v>1726</v>
+      </c>
+      <c r="H29">
+        <f>SUM($B$2:$B29)</f>
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>68</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="C30">
+        <f xml:space="preserve"> D30-10</f>
+        <v>46</v>
+      </c>
+      <c r="D30">
+        <v>56</v>
+      </c>
+      <c r="G30">
+        <f>SUM($C$2:$C30)</f>
+        <v>1772</v>
+      </c>
+      <c r="H30">
+        <f>SUM($B$2:$B30)</f>
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>57</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <f xml:space="preserve"> D31-10</f>
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>55</v>
+      </c>
+      <c r="G31">
+        <f>SUM($C$2:$C31)</f>
+        <v>1817</v>
+      </c>
+      <c r="H31">
+        <f>SUM($B$2:$B31)</f>
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>70</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <f xml:space="preserve"> D32-10</f>
+        <v>45</v>
+      </c>
+      <c r="D32">
+        <v>55</v>
+      </c>
+      <c r="G32">
+        <f>SUM($C$2:$C32)</f>
+        <v>1862</v>
+      </c>
+      <c r="H32">
+        <f>SUM($B$2:$B32)</f>
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>58</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C33">
+        <f xml:space="preserve"> D33-10</f>
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>42</v>
+      </c>
+      <c r="G33">
+        <f>SUM($C$2:$C33)</f>
+        <v>1894</v>
+      </c>
+      <c r="H33">
+        <f>SUM($B$2:$B33)</f>
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>96</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="C34">
+        <f xml:space="preserve"> D34-10</f>
+        <v>87</v>
+      </c>
+      <c r="D34">
+        <v>97</v>
+      </c>
+      <c r="G34">
+        <f>SUM($C$2:$C34)</f>
+        <v>1981</v>
+      </c>
+      <c r="H34">
+        <f>SUM($B$2:$B34)</f>
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>63</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C35">
+        <f xml:space="preserve"> D35-10</f>
+        <v>46</v>
+      </c>
+      <c r="D35">
+        <v>56</v>
+      </c>
+      <c r="G35">
+        <f>SUM($C$2:$C35)</f>
+        <v>2027</v>
+      </c>
+      <c r="H35">
+        <f>SUM($B$2:$B35)</f>
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>74</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <f xml:space="preserve"> D36-10</f>
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>81</v>
+      </c>
+      <c r="G36">
+        <f>SUM($C$2:$C36)</f>
+        <v>2098</v>
+      </c>
+      <c r="H36">
+        <f>SUM($B$2:$B36)</f>
+        <v>2254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>84</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="C37">
+        <f xml:space="preserve"> D37-10</f>
+        <v>64</v>
+      </c>
+      <c r="D37">
+        <v>74</v>
+      </c>
+      <c r="G37">
+        <f>SUM($C$2:$C37)</f>
+        <v>2162</v>
+      </c>
+      <c r="H37">
+        <f>SUM($B$2:$B37)</f>
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>79</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C38">
+        <f xml:space="preserve"> D38-10</f>
+        <v>67</v>
+      </c>
+      <c r="D38">
+        <v>77</v>
+      </c>
+      <c r="G38">
+        <f>SUM($C$2:$C38)</f>
+        <v>2229</v>
+      </c>
+      <c r="H38">
+        <f>SUM($B$2:$B38)</f>
+        <v>2397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finishing webstie - Gameweeks.json saved here without svm
</commit_message>
<xml_diff>
--- a/Statistics/Historical/evaluation.xlsx
+++ b/Statistics/Historical/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicky\Documents\Moneyball\MoneyBall_Code\Statistics\Historical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51291C-29EB-4D18-A7D1-57B1735ED32B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F56C2F8-F509-4468-AFD2-73F7707B9FC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DDEA805C-D17E-4AF5-9BCD-4D2761012DB5}"/>
+    <workbookView minimized="1" xWindow="-8370" yWindow="2790" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{DDEA805C-D17E-4AF5-9BCD-4D2761012DB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
   <si>
     <t>None</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>Gradient Boosting Machines</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>GBM_FIX</t>
+  </si>
+  <si>
+    <t>SVM_FIX</t>
   </si>
 </sst>
 </file>
@@ -3068,14 +3077,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Comparing Random Forest</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparing Random Forests vs GBMs vs SVMs performance in 2018/19 Season</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> to GBM performance in 2018/19 Season</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3155,6 +3159,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="36"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1013124665897929E-16"/>
+                  <c:y val="-1.8242958864282441E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -3165,7 +3175,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-DE7F-4C05-8B42-E3424F0F98B5}"/>
+                  <c16:uniqueId val="{00000005-F567-4F24-864D-9455E94D629E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3198,7 +3208,6 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3348,7 +3357,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DE7F-4C05-8B42-E3424F0F98B5}"/>
+              <c16:uniqueId val="{00000000-F567-4F24-864D-9455E94D629E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3393,7 +3402,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="36"/>
-              <c:dLblPos val="r"/>
+              <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -3403,7 +3412,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-DE7F-4C05-8B42-E3424F0F98B5}"/>
+                  <c16:uniqueId val="{00000004-F567-4F24-864D-9455E94D629E}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3436,7 +3445,6 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3586,12 +3594,248 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DE7F-4C05-8B42-E3424F0F98B5}"/>
+              <c16:uniqueId val="{00000001-F567-4F24-864D-9455E94D629E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gbm_rf!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-F567-4F24-864D-9455E94D629E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>gbm_rf!$I$2:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>698</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>968</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1172</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1236</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1286</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1330</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1414</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1449</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1521</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1582</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1671</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1739</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1801</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1860</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1891</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1946</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2118</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F567-4F24-864D-9455E94D629E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3601,11 +3845,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="555609168"/>
-        <c:axId val="555612048"/>
+        <c:axId val="518442168"/>
+        <c:axId val="518443768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="555609168"/>
+        <c:axId val="518442168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3631,15 +3875,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Gameweek</a:t>
                 </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3672,7 +3910,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3708,7 +3946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555612048"/>
+        <c:crossAx val="518443768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3716,7 +3954,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555612048"/>
+        <c:axId val="518443768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3756,7 +3994,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Total Points</a:t>
                 </a:r>
               </a:p>
@@ -3792,7 +4030,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -3822,7 +4060,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="555609168"/>
+        <c:crossAx val="518442168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3835,7 +4073,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5654,23 +5892,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{794D65F4-BEA0-4470-A8D0-4BB26D78DB0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{460E53BE-99BC-4705-BC20-38ECD0839A48}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7706,32 +7944,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD529F2-74D2-412E-8B56-7C86EFC7D0AC}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="24.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>49</v>
       </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
       <c r="G1" t="s">
         <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>52</v>
       </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>69</v>
       </c>
@@ -7740,11 +7993,18 @@
         <v>59</v>
       </c>
       <c r="C2">
-        <f xml:space="preserve"> D2-10</f>
+        <f t="shared" ref="C2:C38" si="0" xml:space="preserve"> D2-10</f>
         <v>50</v>
       </c>
       <c r="D2">
         <v>60</v>
+      </c>
+      <c r="E2">
+        <v>66</v>
+      </c>
+      <c r="F2">
+        <f>E2-12</f>
+        <v>54</v>
       </c>
       <c r="G2">
         <f>SUM($C$2:$C2)</f>
@@ -7754,21 +8014,32 @@
         <f>SUM($B$2:$B2)</f>
         <v>59</v>
       </c>
+      <c r="I2">
+        <f>SUM($F$2:$F2)</f>
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>72</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B38" si="0">A3-10</f>
+        <f t="shared" ref="B3:B38" si="1">A3-10</f>
         <v>62</v>
       </c>
       <c r="C3">
-        <f xml:space="preserve"> D3-10</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="D3">
         <v>72</v>
+      </c>
+      <c r="E3">
+        <v>66</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F38" si="2">E3-12</f>
+        <v>54</v>
       </c>
       <c r="G3">
         <f>SUM($C$2:$C3)</f>
@@ -7778,21 +8049,32 @@
         <f>SUM($B$2:$B3)</f>
         <v>121</v>
       </c>
+      <c r="I3">
+        <f>SUM($F$2:$F3)</f>
+        <v>108</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>72</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="C4">
-        <f xml:space="preserve"> D4-10</f>
         <v>42</v>
       </c>
       <c r="D4">
         <v>52</v>
+      </c>
+      <c r="E4">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>45</v>
       </c>
       <c r="G4">
         <f>SUM($C$2:$C4)</f>
@@ -7802,21 +8084,32 @@
         <f>SUM($B$2:$B4)</f>
         <v>183</v>
       </c>
+      <c r="I4">
+        <f>SUM($F$2:$F4)</f>
+        <v>153</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>64</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="C5">
-        <f xml:space="preserve"> D5-10</f>
         <v>49</v>
       </c>
       <c r="D5">
         <v>59</v>
+      </c>
+      <c r="E5">
+        <v>104</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
       <c r="G5">
         <f>SUM($C$2:$C5)</f>
@@ -7826,21 +8119,32 @@
         <f>SUM($B$2:$B5)</f>
         <v>237</v>
       </c>
+      <c r="I5">
+        <f>SUM($F$2:$F5)</f>
+        <v>245</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>81</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="C6">
-        <f xml:space="preserve"> D6-10</f>
         <v>67</v>
       </c>
       <c r="D6">
         <v>77</v>
+      </c>
+      <c r="E6">
+        <v>83</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>71</v>
       </c>
       <c r="G6">
         <f>SUM($C$2:$C6)</f>
@@ -7850,21 +8154,32 @@
         <f>SUM($B$2:$B6)</f>
         <v>308</v>
       </c>
+      <c r="I6">
+        <f>SUM($F$2:$F6)</f>
+        <v>316</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>94</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="C7">
-        <f xml:space="preserve"> D7-10</f>
         <v>63</v>
       </c>
       <c r="D7">
         <v>73</v>
+      </c>
+      <c r="E7">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>76</v>
       </c>
       <c r="G7">
         <f>SUM($C$2:$C7)</f>
@@ -7874,21 +8189,32 @@
         <f>SUM($B$2:$B7)</f>
         <v>392</v>
       </c>
+      <c r="I7">
+        <f>SUM($F$2:$F7)</f>
+        <v>392</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>85</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="C8">
-        <f xml:space="preserve"> D8-10</f>
         <v>63</v>
       </c>
       <c r="D8">
         <v>73</v>
+      </c>
+      <c r="E8">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
       <c r="G8">
         <f>SUM($C$2:$C8)</f>
@@ -7898,21 +8224,32 @@
         <f>SUM($B$2:$B8)</f>
         <v>467</v>
       </c>
+      <c r="I8">
+        <f>SUM($F$2:$F8)</f>
+        <v>435</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>82</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C9">
-        <f xml:space="preserve"> D9-10</f>
         <v>47</v>
       </c>
       <c r="D9">
         <v>57</v>
+      </c>
+      <c r="E9">
+        <v>81</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>69</v>
       </c>
       <c r="G9">
         <f>SUM($C$2:$C9)</f>
@@ -7922,20 +8259,31 @@
         <f>SUM($B$2:$B9)</f>
         <v>539</v>
       </c>
+      <c r="I9">
+        <f>SUM($F$2:$F9)</f>
+        <v>504</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>61</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="C10">
-        <f xml:space="preserve"> D10-10</f>
         <v>60</v>
       </c>
       <c r="D10">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>82</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="G10">
@@ -7946,21 +8294,32 @@
         <f>SUM($B$2:$B10)</f>
         <v>590</v>
       </c>
+      <c r="I10">
+        <f>SUM($F$2:$F10)</f>
+        <v>574</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>64</v>
       </c>
       <c r="B11">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="C11">
-        <f xml:space="preserve"> D11-10</f>
-        <v>54</v>
-      </c>
       <c r="D11">
         <v>64</v>
+      </c>
+      <c r="E11">
+        <v>70</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>58</v>
       </c>
       <c r="G11">
         <f>SUM($C$2:$C11)</f>
@@ -7970,21 +8329,32 @@
         <f>SUM($B$2:$B11)</f>
         <v>644</v>
       </c>
+      <c r="I11">
+        <f>SUM($F$2:$F11)</f>
+        <v>632</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>73</v>
       </c>
       <c r="B12">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="C12">
-        <f xml:space="preserve"> D12-10</f>
         <v>58</v>
       </c>
       <c r="D12">
         <v>68</v>
+      </c>
+      <c r="E12">
+        <v>78</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>66</v>
       </c>
       <c r="G12">
         <f>SUM($C$2:$C12)</f>
@@ -7994,21 +8364,32 @@
         <f>SUM($B$2:$B12)</f>
         <v>707</v>
       </c>
+      <c r="I12">
+        <f>SUM($F$2:$F12)</f>
+        <v>698</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>82</v>
       </c>
       <c r="B13">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C13">
-        <f xml:space="preserve"> D13-10</f>
         <v>79</v>
       </c>
       <c r="D13">
         <v>89</v>
+      </c>
+      <c r="E13">
+        <v>88</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>76</v>
       </c>
       <c r="G13">
         <f>SUM($C$2:$C13)</f>
@@ -8018,21 +8399,32 @@
         <f>SUM($B$2:$B13)</f>
         <v>779</v>
       </c>
+      <c r="I13">
+        <f>SUM($F$2:$F13)</f>
+        <v>774</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>84</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="C14">
-        <f xml:space="preserve"> D14-10</f>
         <v>60</v>
       </c>
       <c r="D14">
         <v>70</v>
+      </c>
+      <c r="E14">
+        <v>66</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>54</v>
       </c>
       <c r="G14">
         <f>SUM($C$2:$C14)</f>
@@ -8042,21 +8434,32 @@
         <f>SUM($B$2:$B14)</f>
         <v>853</v>
       </c>
+      <c r="I14">
+        <f>SUM($F$2:$F14)</f>
+        <v>828</v>
+      </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>60</v>
       </c>
       <c r="B15">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="C15">
-        <f xml:space="preserve"> D15-10</f>
         <v>49</v>
       </c>
       <c r="D15">
         <v>59</v>
+      </c>
+      <c r="E15">
+        <v>60</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
       <c r="G15">
         <f>SUM($C$2:$C15)</f>
@@ -8066,21 +8469,32 @@
         <f>SUM($B$2:$B15)</f>
         <v>903</v>
       </c>
+      <c r="I15">
+        <f>SUM($F$2:$F15)</f>
+        <v>876</v>
+      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>82</v>
       </c>
       <c r="B16">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="C16">
-        <f xml:space="preserve"> D16-10</f>
         <v>78</v>
       </c>
       <c r="D16">
         <v>88</v>
+      </c>
+      <c r="E16">
+        <v>104</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>92</v>
       </c>
       <c r="G16">
         <f>SUM($C$2:$C16)</f>
@@ -8090,21 +8504,32 @@
         <f>SUM($B$2:$B16)</f>
         <v>975</v>
       </c>
+      <c r="I16">
+        <f>SUM($F$2:$F16)</f>
+        <v>968</v>
+      </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>75</v>
       </c>
       <c r="B17">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C17">
-        <f xml:space="preserve"> D17-10</f>
         <v>61</v>
       </c>
       <c r="D17">
         <v>71</v>
+      </c>
+      <c r="E17">
+        <v>68</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>56</v>
       </c>
       <c r="G17">
         <f>SUM($C$2:$C17)</f>
@@ -8114,21 +8539,32 @@
         <f>SUM($B$2:$B17)</f>
         <v>1040</v>
       </c>
+      <c r="I17">
+        <f>SUM($F$2:$F17)</f>
+        <v>1024</v>
+      </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>91</v>
       </c>
       <c r="B18">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="C18">
         <f t="shared" si="0"/>
-        <v>81</v>
-      </c>
-      <c r="C18">
-        <f xml:space="preserve"> D18-10</f>
         <v>75</v>
       </c>
       <c r="D18">
         <v>85</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>78</v>
       </c>
       <c r="G18">
         <f>SUM($C$2:$C18)</f>
@@ -8138,21 +8574,32 @@
         <f>SUM($B$2:$B18)</f>
         <v>1121</v>
       </c>
+      <c r="I18">
+        <f>SUM($F$2:$F18)</f>
+        <v>1102</v>
+      </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>79</v>
       </c>
       <c r="B19">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C19">
-        <f xml:space="preserve"> D19-10</f>
         <v>72</v>
       </c>
       <c r="D19">
         <v>82</v>
+      </c>
+      <c r="E19">
+        <v>82</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>70</v>
       </c>
       <c r="G19">
         <f>SUM($C$2:$C19)</f>
@@ -8162,13 +8609,17 @@
         <f>SUM($B$2:$B19)</f>
         <v>1190</v>
       </c>
+      <c r="I19">
+        <f>SUM($F$2:$F19)</f>
+        <v>1172</v>
+      </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>75</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="C20">
@@ -8178,6 +8629,13 @@
       <c r="D20">
         <v>64</v>
       </c>
+      <c r="E20">
+        <v>76</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
       <c r="G20">
         <f>SUM($C$2:$C20)</f>
         <v>1143</v>
@@ -8186,21 +8644,32 @@
         <f>SUM($B$2:$B20)</f>
         <v>1255</v>
       </c>
+      <c r="I20">
+        <f>SUM($F$2:$F20)</f>
+        <v>1236</v>
+      </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>54</v>
       </c>
       <c r="B21">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="C21">
-        <f xml:space="preserve"> D21-10</f>
         <v>55</v>
       </c>
       <c r="D21">
         <v>65</v>
+      </c>
+      <c r="E21">
+        <v>62</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>50</v>
       </c>
       <c r="G21">
         <f>SUM($C$2:$C21)</f>
@@ -8210,21 +8679,32 @@
         <f>SUM($B$2:$B21)</f>
         <v>1299</v>
       </c>
+      <c r="I21">
+        <f>SUM($F$2:$F21)</f>
+        <v>1286</v>
+      </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>72</v>
       </c>
       <c r="B22">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C22">
         <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="C22">
-        <f xml:space="preserve"> D22-10</f>
         <v>66</v>
       </c>
       <c r="D22">
         <v>76</v>
+      </c>
+      <c r="E22">
+        <v>56</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="G22">
         <f>SUM($C$2:$C22)</f>
@@ -8234,21 +8714,32 @@
         <f>SUM($B$2:$B22)</f>
         <v>1361</v>
       </c>
+      <c r="I22">
+        <f>SUM($F$2:$F22)</f>
+        <v>1330</v>
+      </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>72</v>
       </c>
       <c r="B23">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C23">
         <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="C23">
-        <f xml:space="preserve"> D23-10</f>
         <v>67</v>
       </c>
       <c r="D23">
         <v>77</v>
+      </c>
+      <c r="E23">
+        <v>56</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="G23">
         <f>SUM($C$2:$C23)</f>
@@ -8258,21 +8749,32 @@
         <f>SUM($B$2:$B23)</f>
         <v>1423</v>
       </c>
+      <c r="I23">
+        <f>SUM($F$2:$F23)</f>
+        <v>1374</v>
+      </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>75</v>
       </c>
       <c r="B24">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C24">
         <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C24">
-        <f xml:space="preserve"> D24-10</f>
         <v>62</v>
       </c>
       <c r="D24">
         <v>72</v>
+      </c>
+      <c r="E24">
+        <v>52</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="G24">
         <f>SUM($C$2:$C24)</f>
@@ -8282,21 +8784,32 @@
         <f>SUM($B$2:$B24)</f>
         <v>1488</v>
       </c>
+      <c r="I24">
+        <f>SUM($F$2:$F24)</f>
+        <v>1414</v>
+      </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>76</v>
       </c>
       <c r="B25">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="C25">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="C25">
-        <f xml:space="preserve"> D25-10</f>
         <v>73</v>
       </c>
       <c r="D25">
         <v>83</v>
+      </c>
+      <c r="E25">
+        <v>47</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
       <c r="G25">
         <f>SUM($C$2:$C25)</f>
@@ -8306,21 +8819,32 @@
         <f>SUM($B$2:$B25)</f>
         <v>1554</v>
       </c>
+      <c r="I25">
+        <f>SUM($F$2:$F25)</f>
+        <v>1449</v>
+      </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>88</v>
       </c>
       <c r="B26">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C26">
         <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="C26">
-        <f xml:space="preserve"> D26-10</f>
         <v>74</v>
       </c>
       <c r="D26">
         <v>84</v>
+      </c>
+      <c r="E26">
+        <v>84</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>72</v>
       </c>
       <c r="G26">
         <f>SUM($C$2:$C26)</f>
@@ -8330,21 +8854,32 @@
         <f>SUM($B$2:$B26)</f>
         <v>1632</v>
       </c>
+      <c r="I26">
+        <f>SUM($F$2:$F26)</f>
+        <v>1521</v>
+      </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>84</v>
       </c>
       <c r="B27">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="C27">
-        <f xml:space="preserve"> D27-10</f>
         <v>68</v>
       </c>
       <c r="D27">
         <v>78</v>
+      </c>
+      <c r="E27">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>61</v>
       </c>
       <c r="G27">
         <f>SUM($C$2:$C27)</f>
@@ -8354,21 +8889,32 @@
         <f>SUM($B$2:$B27)</f>
         <v>1706</v>
       </c>
+      <c r="I27">
+        <f>SUM($F$2:$F27)</f>
+        <v>1582</v>
+      </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>88</v>
       </c>
       <c r="B28">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="C28">
         <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="C28">
-        <f xml:space="preserve"> D28-10</f>
         <v>72</v>
       </c>
       <c r="D28">
         <v>82</v>
+      </c>
+      <c r="E28">
+        <v>68</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>56</v>
       </c>
       <c r="G28">
         <f>SUM($C$2:$C28)</f>
@@ -8378,21 +8924,32 @@
         <f>SUM($B$2:$B28)</f>
         <v>1784</v>
       </c>
+      <c r="I28">
+        <f>SUM($F$2:$F28)</f>
+        <v>1638</v>
+      </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>64</v>
       </c>
       <c r="B29">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C29">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="C29">
-        <f xml:space="preserve"> D29-10</f>
         <v>46</v>
       </c>
       <c r="D29">
         <v>56</v>
+      </c>
+      <c r="E29">
+        <v>45</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
       <c r="G29">
         <f>SUM($C$2:$C29)</f>
@@ -8402,21 +8959,32 @@
         <f>SUM($B$2:$B29)</f>
         <v>1838</v>
       </c>
+      <c r="I29">
+        <f>SUM($F$2:$F29)</f>
+        <v>1671</v>
+      </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>68</v>
       </c>
       <c r="B30">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C30">
         <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C30">
-        <f xml:space="preserve"> D30-10</f>
         <v>46</v>
       </c>
       <c r="D30">
         <v>56</v>
+      </c>
+      <c r="E30">
+        <v>80</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>68</v>
       </c>
       <c r="G30">
         <f>SUM($C$2:$C30)</f>
@@ -8426,21 +8994,32 @@
         <f>SUM($B$2:$B30)</f>
         <v>1896</v>
       </c>
+      <c r="I30">
+        <f>SUM($F$2:$F30)</f>
+        <v>1739</v>
+      </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>57</v>
       </c>
       <c r="B31">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="C31">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="C31">
-        <f xml:space="preserve"> D31-10</f>
         <v>45</v>
       </c>
       <c r="D31">
         <v>55</v>
+      </c>
+      <c r="E31">
+        <v>74</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>62</v>
       </c>
       <c r="G31">
         <f>SUM($C$2:$C31)</f>
@@ -8450,21 +9029,32 @@
         <f>SUM($B$2:$B31)</f>
         <v>1943</v>
       </c>
+      <c r="I31">
+        <f>SUM($F$2:$F31)</f>
+        <v>1801</v>
+      </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>70</v>
       </c>
       <c r="B32">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C32">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C32">
-        <f xml:space="preserve"> D32-10</f>
         <v>45</v>
       </c>
       <c r="D32">
         <v>55</v>
+      </c>
+      <c r="E32">
+        <v>71</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>59</v>
       </c>
       <c r="G32">
         <f>SUM($C$2:$C32)</f>
@@ -8474,21 +9064,32 @@
         <f>SUM($B$2:$B32)</f>
         <v>2003</v>
       </c>
+      <c r="I32">
+        <f>SUM($F$2:$F32)</f>
+        <v>1860</v>
+      </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>58</v>
       </c>
       <c r="B33">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="C33">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="C33">
-        <f xml:space="preserve"> D33-10</f>
         <v>32</v>
       </c>
       <c r="D33">
         <v>42</v>
+      </c>
+      <c r="E33">
+        <v>43</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="G33">
         <f>SUM($C$2:$C33)</f>
@@ -8498,21 +9099,32 @@
         <f>SUM($B$2:$B33)</f>
         <v>2051</v>
       </c>
+      <c r="I33">
+        <f>SUM($F$2:$F33)</f>
+        <v>1891</v>
+      </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>96</v>
       </c>
       <c r="B34">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="C34">
         <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-      <c r="C34">
-        <f xml:space="preserve"> D34-10</f>
         <v>87</v>
       </c>
       <c r="D34">
         <v>97</v>
+      </c>
+      <c r="E34">
+        <v>67</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>55</v>
       </c>
       <c r="G34">
         <f>SUM($C$2:$C34)</f>
@@ -8522,21 +9134,32 @@
         <f>SUM($B$2:$B34)</f>
         <v>2137</v>
       </c>
+      <c r="I34">
+        <f>SUM($F$2:$F34)</f>
+        <v>1946</v>
+      </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>63</v>
       </c>
       <c r="B35">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="C35">
         <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="C35">
-        <f xml:space="preserve"> D35-10</f>
         <v>46</v>
       </c>
       <c r="D35">
         <v>56</v>
+      </c>
+      <c r="E35">
+        <v>77</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>65</v>
       </c>
       <c r="G35">
         <f>SUM($C$2:$C35)</f>
@@ -8546,21 +9169,32 @@
         <f>SUM($B$2:$B35)</f>
         <v>2190</v>
       </c>
+      <c r="I35">
+        <f>SUM($F$2:$F35)</f>
+        <v>2011</v>
+      </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>74</v>
       </c>
       <c r="B36">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C36">
         <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C36">
-        <f xml:space="preserve"> D36-10</f>
         <v>71</v>
       </c>
       <c r="D36">
         <v>81</v>
+      </c>
+      <c r="E36">
+        <v>81</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>69</v>
       </c>
       <c r="G36">
         <f>SUM($C$2:$C36)</f>
@@ -8570,21 +9204,32 @@
         <f>SUM($B$2:$B36)</f>
         <v>2254</v>
       </c>
+      <c r="I36">
+        <f>SUM($F$2:$F36)</f>
+        <v>2080</v>
+      </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>84</v>
       </c>
       <c r="B37">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="C37">
         <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="C37">
-        <f xml:space="preserve"> D37-10</f>
         <v>64</v>
       </c>
       <c r="D37">
         <v>74</v>
+      </c>
+      <c r="E37">
+        <v>50</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="G37">
         <f>SUM($C$2:$C37)</f>
@@ -8594,21 +9239,32 @@
         <f>SUM($B$2:$B37)</f>
         <v>2328</v>
       </c>
+      <c r="I37">
+        <f>SUM($F$2:$F37)</f>
+        <v>2118</v>
+      </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>79</v>
       </c>
       <c r="B38">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="C38">
         <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C38">
-        <f xml:space="preserve"> D38-10</f>
         <v>67</v>
       </c>
       <c r="D38">
         <v>77</v>
+      </c>
+      <c r="E38">
+        <v>96</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>84</v>
       </c>
       <c r="G38">
         <f>SUM($C$2:$C38)</f>
@@ -8617,6 +9273,30 @@
       <c r="H38">
         <f>SUM($B$2:$B38)</f>
         <v>2397</v>
+      </c>
+      <c r="I38">
+        <f>SUM($F$2:$F38)</f>
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f>AVERAGE(B2:B38)</f>
+        <v>64.78378378378379</v>
+      </c>
+      <c r="C40">
+        <f>AVERAGE(C2:C38)</f>
+        <v>60.243243243243242</v>
+      </c>
+      <c r="F40">
+        <f>AVERAGE(F2:F38)</f>
+        <v>59.513513513513516</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E42">
+        <f>2314/38</f>
+        <v>60.89473684210526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>